<commit_message>
W13 Wednesday Commit 1
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755C12A5-3F18-4C08-B240-841F0E691607}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC29043B-AC48-489D-9E86-896386BA1C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="24573" windowHeight="14586" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -70,15 +70,32 @@
   <si>
     <t>Leaf5</t>
   </si>
+  <si>
+    <t>Leaf 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,9 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +443,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -536,30 +555,120 @@
       <c r="A6" s="1">
         <v>44015</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>44016</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>44017</v>
       </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>44018</v>
       </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>44019</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>44020</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -667,7 +776,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -779,30 +888,120 @@
       <c r="A6" s="1">
         <v>44015</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>44016</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>44017</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>44018</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>44019</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>44020</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
@@ -907,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B3BC5-B675-4141-913B-1E50AEE555B7}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -918,7 +1117,7 @@
     <col min="1" max="1" width="9.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -937,8 +1136,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>44011</v>
       </c>
@@ -958,7 +1160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>44012</v>
       </c>
@@ -978,7 +1180,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>44013</v>
       </c>
@@ -998,7 +1200,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>44014</v>
       </c>
@@ -1018,57 +1220,156 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>44015</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>44016</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B7">
+        <v>19.5</v>
+      </c>
+      <c r="C7">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>44017</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>22.5</v>
+      </c>
+      <c r="F8">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>44018</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B9">
+        <v>19.5</v>
+      </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="E9">
+        <v>22.5</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>44019</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>18.5</v>
+      </c>
+      <c r="D10">
+        <v>7.5</v>
+      </c>
+      <c r="E10">
+        <v>21.75</v>
+      </c>
+      <c r="F10">
+        <v>12.5</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>44020</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>19.34</v>
+      </c>
+      <c r="D11">
+        <v>7.25</v>
+      </c>
+      <c r="E11">
+        <v>21.5</v>
+      </c>
+      <c r="F11">
+        <v>12.5</v>
+      </c>
+      <c r="G11">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>44021</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
       </c>
@@ -1150,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584FC315-4067-4CDA-9E22-E3EDB6840305}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1161,7 +1462,7 @@
     <col min="1" max="1" width="9.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1180,8 +1481,11 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>44011</v>
       </c>
@@ -1201,7 +1505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>44012</v>
       </c>
@@ -1221,7 +1525,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>44013</v>
       </c>
@@ -1241,7 +1545,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>44014</v>
       </c>
@@ -1261,57 +1565,156 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>44015</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>13.5</v>
+      </c>
+      <c r="D6">
+        <v>18.5</v>
+      </c>
+      <c r="E6">
+        <v>24.5</v>
+      </c>
+      <c r="F6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>44016</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>20.75</v>
+      </c>
+      <c r="E7">
+        <v>24</v>
+      </c>
+      <c r="F7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>44017</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>13.5</v>
+      </c>
+      <c r="D8">
+        <v>21.5</v>
+      </c>
+      <c r="E8">
+        <v>23.75</v>
+      </c>
+      <c r="F8">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>44018</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B9">
+        <v>24.5</v>
+      </c>
+      <c r="C9" s="3">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>22.5</v>
+      </c>
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>24.5</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>44019</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B10">
+        <v>24.75</v>
+      </c>
+      <c r="C10">
+        <v>13.25</v>
+      </c>
+      <c r="D10">
+        <v>23.25</v>
+      </c>
+      <c r="E10">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>24.5</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>44020</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="B11">
+        <v>24.25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>24.18</v>
+      </c>
+      <c r="E11">
+        <v>24</v>
+      </c>
+      <c r="F11">
+        <v>24.5</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>44021</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
       </c>
@@ -1388,5 +1791,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
W14 Monday Commit 1
fixed links in readme, update for excel sheet (does not include today, will let plants get more sun before measuring them), finished timecard for week 13
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC29043B-AC48-489D-9E86-896386BA1C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027F1518-99DB-4836-9C1B-503C933CC48B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="24573" windowHeight="14586" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -675,20 +675,80 @@
       <c r="A12" s="1">
         <v>44021</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -776,7 +836,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1008,20 +1068,80 @@
       <c r="A12" s="1">
         <v>44021</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
@@ -1109,7 +1229,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1353,20 +1473,92 @@
       <c r="A12" s="1">
         <v>44021</v>
       </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>18.75</v>
+      </c>
+      <c r="D12">
+        <v>6.5</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>12</v>
+      </c>
+      <c r="G12">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>19.25</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>22.5</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
+      <c r="B14">
+        <v>19.75</v>
+      </c>
+      <c r="C14">
+        <v>19.25</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>22.5</v>
+      </c>
+      <c r="F14">
+        <v>12.75</v>
+      </c>
+      <c r="G14">
+        <v>11.25</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
+      </c>
+      <c r="B15">
+        <v>19.75</v>
+      </c>
+      <c r="C15">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>6.5</v>
+      </c>
+      <c r="E15">
+        <v>22.5</v>
+      </c>
+      <c r="F15">
+        <v>12.25</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
@@ -1451,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584FC315-4067-4CDA-9E22-E3EDB6840305}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1698,21 +1890,87 @@
       <c r="A12" s="1">
         <v>44021</v>
       </c>
+      <c r="B12">
+        <v>24.5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <v>24</v>
+      </c>
+      <c r="F12">
+        <v>24.5</v>
+      </c>
+      <c r="G12">
+        <v>8.5</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
+      <c r="B13">
+        <v>24.25</v>
+      </c>
+      <c r="C13">
+        <v>11.75</v>
+      </c>
+      <c r="D13">
+        <v>25.5</v>
+      </c>
+      <c r="E13">
+        <v>24</v>
+      </c>
+      <c r="F13">
+        <v>24.75</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
+      <c r="B14">
+        <v>24.5</v>
+      </c>
+      <c r="D14">
+        <v>25.5</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>24.75</v>
+      </c>
+      <c r="G14">
+        <v>14.25</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
       </c>
+      <c r="B15">
+        <v>24.5</v>
+      </c>
+      <c r="D15">
+        <v>25.75</v>
+      </c>
+      <c r="E15">
+        <v>23.75</v>
+      </c>
+      <c r="F15">
+        <v>24.5</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
@@ -1787,6 +2045,11 @@
     <row r="30" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A31" s="1">
+        <v>44040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
W14 Monday Commit 4
Updated timecard, excel sheet, and chapter 6 report.
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027F1518-99DB-4836-9C1B-503C933CC48B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376BAFB7-5118-4423-BC4D-D82A025D4AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="24573" windowHeight="14586" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -754,6 +754,21 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
@@ -836,7 +851,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1147,6 +1162,21 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
@@ -1229,7 +1259,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1564,6 +1594,24 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>19.5</v>
+      </c>
+      <c r="D16">
+        <v>6.5</v>
+      </c>
+      <c r="E16">
+        <v>22.5</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
@@ -1646,7 +1694,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1976,6 +2024,21 @@
       <c r="A16" s="1">
         <v>44025</v>
       </c>
+      <c r="B16">
+        <v>24.75</v>
+      </c>
+      <c r="D16">
+        <v>26</v>
+      </c>
+      <c r="E16">
+        <v>24</v>
+      </c>
+      <c r="F16">
+        <v>24.5</v>
+      </c>
+      <c r="G16">
+        <v>16.25</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A17" s="1">

</xml_diff>

<commit_message>
W14 Wednesday Commit 1
updated chapter  6 report 1; garden excel sheet; garden observation sheet; timecard.
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376BAFB7-5118-4423-BC4D-D82A025D4AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A57D9D-AE18-4CD9-A06E-983F2A867CAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="24573" windowHeight="14586" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
+    <workbookView xWindow="32835" yWindow="-15135" windowWidth="15300" windowHeight="12945" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Pansies Alive" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Leaf 6</t>
+  </si>
+  <si>
+    <t>Leaf 7</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -771,72 +774,102 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>44026</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>44027</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>44028</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>44034</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>44036</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>44037</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
       </c>
@@ -851,7 +884,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1179,72 +1212,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>44026</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>44027</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>44028</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>44034</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>44036</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>44037</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
       </c>
@@ -1259,7 +1322,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1614,72 +1677,108 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>44026</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B17">
+        <v>19.75</v>
+      </c>
+      <c r="C17">
+        <v>19.5</v>
+      </c>
+      <c r="D17">
+        <v>6.5</v>
+      </c>
+      <c r="E17">
+        <v>22.25</v>
+      </c>
+      <c r="F17">
+        <v>12.5</v>
+      </c>
+      <c r="G17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>44027</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>19.75</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>22.5</v>
+      </c>
+      <c r="F18">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>44028</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>44034</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>44036</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>44037</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
       </c>
@@ -1691,10 +1790,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584FC315-4067-4CDA-9E22-E3EDB6840305}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1702,7 +1801,7 @@
     <col min="1" max="1" width="9.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1724,8 +1823,11 @@
       <c r="G1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>44011</v>
       </c>
@@ -1745,7 +1847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>44012</v>
       </c>
@@ -1765,7 +1867,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>44013</v>
       </c>
@@ -1785,7 +1887,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>44014</v>
       </c>
@@ -1805,7 +1907,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>44015</v>
       </c>
@@ -1825,7 +1927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>44016</v>
       </c>
@@ -1845,7 +1947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>44017</v>
       </c>
@@ -1865,7 +1967,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>44018</v>
       </c>
@@ -1888,7 +1990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>44019</v>
       </c>
@@ -1911,7 +2013,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>44020</v>
       </c>
@@ -1934,7 +2036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>44021</v>
       </c>
@@ -1957,7 +2059,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
@@ -1980,7 +2082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
@@ -2000,7 +2102,7 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
       </c>
@@ -2020,7 +2122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
       </c>
@@ -2040,77 +2142,113 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>44026</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B17">
+        <v>24.75</v>
+      </c>
+      <c r="D17">
+        <v>26.5</v>
+      </c>
+      <c r="E17">
+        <v>24.25</v>
+      </c>
+      <c r="F17">
+        <v>24.75</v>
+      </c>
+      <c r="G17">
+        <v>18.25</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>44027</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="B18">
+        <v>24.5</v>
+      </c>
+      <c r="D18">
+        <v>26.25</v>
+      </c>
+      <c r="E18">
+        <v>24.25</v>
+      </c>
+      <c r="F18">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>20.5</v>
+      </c>
+      <c r="H18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>44028</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>44034</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>44036</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>44037</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31" s="1">
         <v>44040</v>
       </c>

</xml_diff>

<commit_message>
W15 Tuesday Commit 1
Final timecard from week 14.  Updated excel sheet.  Updated chapter report.  Updated README.
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F40FF4A-E7CC-41E3-9F58-FB0306BF984A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9821339-044E-4559-B048-374649B61501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32835" yWindow="-15135" windowWidth="15300" windowHeight="12945" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
+    <workbookView xWindow="25680" yWindow="-14010" windowWidth="19200" windowHeight="10515" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Pansies Alive" sheetId="1" r:id="rId1"/>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9442565D-768E-4D8E-AB75-7B5EDC6C2F4C}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -838,25 +838,100 @@
       <c r="A20" s="1">
         <v>44029</v>
       </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -898,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590A878F-CD56-4453-AEDF-254594B2B878}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1291,25 +1366,100 @@
       <c r="A20" s="1">
         <v>44029</v>
       </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -1351,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B3BC5-B675-4141-913B-1E50AEE555B7}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1786,25 +1936,112 @@
       <c r="A20" s="1">
         <v>44029</v>
       </c>
+      <c r="B20">
+        <v>19.5</v>
+      </c>
+      <c r="C20">
+        <v>19.5</v>
+      </c>
+      <c r="D20">
+        <v>6.25</v>
+      </c>
+      <c r="E20">
+        <v>22.75</v>
+      </c>
+      <c r="F20">
+        <v>11.75</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
+      <c r="B21">
+        <v>19.75</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>6.25</v>
+      </c>
+      <c r="E21">
+        <v>22.5</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
+      </c>
+      <c r="G21">
+        <v>16.5</v>
+      </c>
+      <c r="H21">
+        <v>3.25</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
+      <c r="B22">
+        <v>19.5</v>
+      </c>
+      <c r="C22">
+        <v>19.5</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>22.5</v>
+      </c>
+      <c r="F22">
+        <v>11.75</v>
+      </c>
+      <c r="H22">
+        <v>3.25</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
+      <c r="B23">
+        <v>19.25</v>
+      </c>
+      <c r="C23">
+        <v>19.5</v>
+      </c>
+      <c r="F23">
+        <v>11.75</v>
+      </c>
+      <c r="G23">
+        <v>19</v>
+      </c>
+      <c r="H23">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
+      </c>
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>19.5</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+      <c r="H24">
+        <v>5.75</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.5">
@@ -1846,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584FC315-4067-4CDA-9E22-E3EDB6840305}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2269,25 +2506,115 @@
       <c r="A20" s="1">
         <v>44029</v>
       </c>
+      <c r="B20">
+        <v>24.5</v>
+      </c>
+      <c r="D20">
+        <v>26.75</v>
+      </c>
+      <c r="E20">
+        <v>24.5</v>
+      </c>
+      <c r="F20">
+        <v>24.75</v>
+      </c>
+      <c r="G20">
+        <v>22.34</v>
+      </c>
+      <c r="H20">
+        <v>3.75</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
+      <c r="B21">
+        <v>24.75</v>
+      </c>
+      <c r="D21">
+        <v>26.5</v>
+      </c>
+      <c r="E21">
+        <v>24</v>
+      </c>
+      <c r="F21">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>7.75</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
+      <c r="B22">
+        <v>24.25</v>
+      </c>
+      <c r="D22">
+        <v>26.75</v>
+      </c>
+      <c r="E22">
+        <v>24</v>
+      </c>
+      <c r="F22">
+        <v>24.5</v>
+      </c>
+      <c r="G22">
+        <v>23.5</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <v>26.75</v>
+      </c>
+      <c r="E23">
+        <v>24</v>
+      </c>
+      <c r="F23">
+        <v>24.5</v>
+      </c>
+      <c r="G23">
+        <v>24</v>
+      </c>
+      <c r="H23">
+        <v>10.25</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
+      </c>
+      <c r="B24">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>26.75</v>
+      </c>
+      <c r="E24">
+        <v>24.5</v>
+      </c>
+      <c r="F24">
+        <v>24.75</v>
+      </c>
+      <c r="G24">
+        <v>24.25</v>
+      </c>
+      <c r="H24">
+        <v>12.5</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
W15 Thursday Commit 1
Updated timecard; updated garden data collection.
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2CFD27-2EB5-4C65-8F92-DF7B8BE1ACC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51056488-4CEE-467D-A8A9-1E8DEDFB3D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25680" yWindow="-14010" windowWidth="19200" windowHeight="10515" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -957,6 +957,21 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
@@ -989,7 +1004,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1500,6 +1515,21 @@
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
@@ -1532,7 +1562,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2087,6 +2117,9 @@
       <c r="F25">
         <v>11.75</v>
       </c>
+      <c r="G25">
+        <v>17</v>
+      </c>
       <c r="H25">
         <v>7</v>
       </c>
@@ -2094,6 +2127,18 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
+      </c>
+      <c r="C26">
+        <v>19.75</v>
+      </c>
+      <c r="F26">
+        <v>12</v>
+      </c>
+      <c r="G26">
+        <v>17</v>
+      </c>
+      <c r="H26">
+        <v>7.75</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.5">
@@ -2126,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584FC315-4067-4CDA-9E22-E3EDB6840305}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2684,6 +2729,21 @@
       <c r="A26" s="1">
         <v>44035</v>
       </c>
+      <c r="D26">
+        <v>27</v>
+      </c>
+      <c r="E26">
+        <v>24.5</v>
+      </c>
+      <c r="F26">
+        <v>24.5</v>
+      </c>
+      <c r="G26">
+        <v>24.5</v>
+      </c>
+      <c r="H26">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" s="1">

</xml_diff>

<commit_message>
W16 Thursday Commit 1
</commit_message>
<xml_diff>
--- a/data_sources/Garden Practicum.xlsx
+++ b/data_sources/Garden Practicum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Persimmon\Documents\GitHub\Statistics-ILC\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0F98AB-D45B-40DC-97B8-204177FBBC8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0156CF-819A-4020-ACB4-BC6190A2AC66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="-14010" windowWidth="19200" windowHeight="10515" activeTab="1" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
+    <workbookView xWindow="9660" yWindow="-16320" windowWidth="38640" windowHeight="16440" activeTab="3" xr2:uid="{62565F06-D595-4083-8EC0-1415BBCB31B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Pansies Alive" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Pansy5</t>
+  </si>
+  <si>
+    <t>Leaf6</t>
+  </si>
+  <si>
+    <t>Leaf7</t>
+  </si>
+  <si>
+    <t>Leaf8</t>
   </si>
 </sst>
 </file>
@@ -443,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9442565D-768E-4D8E-AB75-7B5EDC6C2F4C}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -998,15 +1007,80 @@
       <c r="A28" s="1">
         <v>44037</v>
       </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
+      <c r="B29">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
+      </c>
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A31" s="1">
+        <v>44040</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1016,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{590A878F-CD56-4453-AEDF-254594B2B878}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1571,15 +1645,80 @@
       <c r="A28" s="1">
         <v>44037</v>
       </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A31" s="1">
+        <v>44040</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1589,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8B3BC5-B675-4141-913B-1E50AEE555B7}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2192,15 +2331,68 @@
       <c r="A28" s="1">
         <v>44037</v>
       </c>
+      <c r="C28">
+        <v>19.75</v>
+      </c>
+      <c r="F28">
+        <v>12</v>
+      </c>
+      <c r="G28">
+        <v>17.5</v>
+      </c>
+      <c r="H28">
+        <v>9</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
+      <c r="C29">
+        <v>20.25</v>
+      </c>
+      <c r="F29">
+        <v>12</v>
+      </c>
+      <c r="G29">
+        <v>17.5</v>
+      </c>
+      <c r="H29">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
+      </c>
+      <c r="C30">
+        <v>19.5</v>
+      </c>
+      <c r="F30">
+        <v>11</v>
+      </c>
+      <c r="G30">
+        <v>17.5</v>
+      </c>
+      <c r="H30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A31" s="1">
+        <v>44040</v>
+      </c>
+      <c r="C31">
+        <v>20.25</v>
+      </c>
+      <c r="F31">
+        <v>11.5</v>
+      </c>
+      <c r="G31">
+        <v>17.75</v>
+      </c>
+      <c r="H31">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2211,10 +2403,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584FC315-4067-4CDA-9E22-E3EDB6840305}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2222,7 +2414,7 @@
     <col min="1" max="1" width="9.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2242,13 +2434,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>44011</v>
       </c>
@@ -2268,7 +2463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>44012</v>
       </c>
@@ -2288,7 +2483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>44013</v>
       </c>
@@ -2308,7 +2503,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>44014</v>
       </c>
@@ -2328,7 +2523,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>44015</v>
       </c>
@@ -2348,7 +2543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>44016</v>
       </c>
@@ -2368,7 +2563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>44017</v>
       </c>
@@ -2388,7 +2583,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
         <v>44018</v>
       </c>
@@ -2411,7 +2606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
         <v>44019</v>
       </c>
@@ -2434,7 +2629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
         <v>44020</v>
       </c>
@@ -2457,7 +2652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
         <v>44021</v>
       </c>
@@ -2480,7 +2675,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
         <v>44022</v>
       </c>
@@ -2503,7 +2698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
         <v>44023</v>
       </c>
@@ -2523,7 +2718,7 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
         <v>44024</v>
       </c>
@@ -2543,7 +2738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
         <v>44025</v>
       </c>
@@ -2563,7 +2758,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
         <v>44026</v>
       </c>
@@ -2586,7 +2781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
         <v>44027</v>
       </c>
@@ -2609,7 +2804,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
         <v>44028</v>
       </c>
@@ -2632,7 +2827,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
         <v>44029</v>
       </c>
@@ -2655,7 +2850,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
         <v>44030</v>
       </c>
@@ -2678,7 +2873,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
         <v>44031</v>
       </c>
@@ -2701,7 +2896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
         <v>44032</v>
       </c>
@@ -2724,7 +2919,7 @@
         <v>10.25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
         <v>44033</v>
       </c>
@@ -2747,7 +2942,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
         <v>44034</v>
       </c>
@@ -2767,7 +2962,7 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
         <v>44035</v>
       </c>
@@ -2787,7 +2982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
         <v>44036</v>
       </c>
@@ -2807,24 +3002,90 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
         <v>44037</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28">
+        <v>24.5</v>
+      </c>
+      <c r="F28">
+        <v>24.75</v>
+      </c>
+      <c r="G28">
+        <v>24.75</v>
+      </c>
+      <c r="H28">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
         <v>44038</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>24</v>
+      </c>
+      <c r="F29">
+        <v>24.5</v>
+      </c>
+      <c r="G29">
+        <v>25.5</v>
+      </c>
+      <c r="H29">
+        <v>17.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
         <v>44039</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="D30">
+        <v>27</v>
+      </c>
+      <c r="E30">
+        <v>24</v>
+      </c>
+      <c r="F30">
+        <v>25</v>
+      </c>
+      <c r="G30">
+        <v>25</v>
+      </c>
+      <c r="H30">
+        <v>18.25</v>
+      </c>
+      <c r="I30">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" s="1">
         <v>44040</v>
+      </c>
+      <c r="D31">
+        <v>27</v>
+      </c>
+      <c r="E31">
+        <v>24.5</v>
+      </c>
+      <c r="F31">
+        <v>25.5</v>
+      </c>
+      <c r="G31">
+        <v>25</v>
+      </c>
+      <c r="H31">
+        <v>18.5</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>